<commit_message>
fixed drift check indexing and string literals deprecation
</commit_message>
<xml_diff>
--- a/test_data/lasercalc_example_export_BCR-2G.xlsx
+++ b/test_data/lasercalc_example_export_BCR-2G.xlsx
@@ -16854,7 +16854,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC21"/>
+  <dimension ref="A1:AP21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16945,67 +16945,132 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>7Li_se</t>
+          <t>7Li_exterr</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>24Mg_se</t>
+          <t>24Mg_exterr</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>27Al_se</t>
+          <t>27Al_exterr</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>29Si_se</t>
+          <t>29Si_exterr</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>43Ca_se</t>
+          <t>43Ca_exterr</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>48Ti_se</t>
+          <t>48Ti_exterr</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>57Fe_se</t>
+          <t>57Fe_exterr</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>88Sr_se</t>
+          <t>88Sr_exterr</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>138Ba_se</t>
+          <t>138Ba_exterr</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>139La_se</t>
+          <t>139La_exterr</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>140Ce_se</t>
+          <t>140Ce_exterr</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>153Eu_se</t>
+          <t>153Eu_exterr</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>208Pb_se</t>
+          <t>208Pb_exterr</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>7Li_interr</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>24Mg_interr</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>27Al_interr</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>29Si_interr</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>43Ca_interr</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>48Ti_interr</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>57Fe_interr</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>88Sr_interr</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>138Ba_interr</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>139La_interr</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>140Ce_interr</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>153Eu_interr</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>208Pb_interr</t>
         </is>
       </c>
     </row>
@@ -17103,6 +17168,45 @@
       <c r="AC2" t="n">
         <v>0.6644538762439895</v>
       </c>
+      <c r="AD2" t="n">
+        <v>2.99884954517325</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>48.89894113114184</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>2054.470196328495</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>288.3988600395895</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>111.107842412584</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>611.0676505325631</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1.687864375368129</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>9.692056101501699</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>1.221923406170256</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>2.317004528629859</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.0648134729050522</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.6622267791898836</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -17198,6 +17302,45 @@
       <c r="AC3" t="n">
         <v>0.5331471995062036</v>
       </c>
+      <c r="AD3" t="n">
+        <v>3.063484187314715</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>15.96768893768607</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>2052.029463518423</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>255.7431783670662</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>112.5062105657118</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>611.8986831716545</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1.683607805334793</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>9.458524230717785</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>1.201585809031792</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>2.279990595576796</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.06154961528371558</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.5305181401048905</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -17293,6 +17436,45 @@
       <c r="AC4" t="n">
         <v>0.5566525763285903</v>
       </c>
+      <c r="AD4" t="n">
+        <v>3.013958139085485</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>17.16654268608011</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>2081.344579068213</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>260.5078612846243</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>115.0057949850195</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>625.0929332459941</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>1.737508862968636</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>9.851096965883187</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>1.256847508806852</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>2.372410924149129</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.06488106396811474</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0.5540364298939671</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -17388,6 +17570,45 @@
       <c r="AC5" t="n">
         <v>0.5448124450633746</v>
       </c>
+      <c r="AD5" t="n">
+        <v>3.051264093685064</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>16.41450068572062</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>2071.437042740539</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>263.2575557525885</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>114.6491165379979</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>627.9086184498912</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>1.724226175882502</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>9.815957466681054</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>1.245431961277169</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>2.338513401763503</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.0639069417626261</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.5421317640714155</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -17483,6 +17704,45 @@
       <c r="AC6" t="n">
         <v>0.5678599065224346</v>
       </c>
+      <c r="AD6" t="n">
+        <v>3.097347602283943</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>16.72955856561553</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>2094.771179519221</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>266.1213050856113</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>116.7266881221813</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>628.3835748407728</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>1.748732673360951</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>10.00092050331233</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>1.261438857762394</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>2.390571890564169</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.06643033124233753</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.5650628078403056</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -17578,6 +17838,45 @@
       <c r="AC7" t="n">
         <v>0.5662956448359023</v>
       </c>
+      <c r="AD7" t="n">
+        <v>3.148340124627654</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>16.61207386922101</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>2079.084315315049</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>267.5037539872917</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>116.6716110198576</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>637.1359167474503</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>1.752277281380337</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>9.983931239484622</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>1.257580190222183</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>2.412926728357637</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0.0668838391239651</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0.5635078113309172</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -17673,6 +17972,45 @@
       <c r="AC8" t="n">
         <v>0.5625624787611712</v>
       </c>
+      <c r="AD8" t="n">
+        <v>3.159637294009065</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>16.85472657989437</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>2112.818711005713</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>267.0079023070129</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>118.4358305629869</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>641.1284596286813</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>1.795034333221278</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>10.17228462369724</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>1.281551318539665</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>2.445148069826108</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>0.06414456886466371</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>0.5597793824161401</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -17768,6 +18106,45 @@
       <c r="AC9" t="n">
         <v>0.5622388184462893</v>
       </c>
+      <c r="AD9" t="n">
+        <v>3.086683972577208</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>16.69125305716587</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>2087.533201793496</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>263.6378708495386</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>118.3240095599956</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>638.0907190648031</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>1.76300325192444</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>10.0136251965347</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>1.262837401112847</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>2.42992066217099</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>0.06487385524833321</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>0.5594649593380577</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -17863,6 +18240,45 @@
       <c r="AC10" t="n">
         <v>0.549423481163317</v>
       </c>
+      <c r="AD10" t="n">
+        <v>3.112864385663483</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>16.67851658484326</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>2086.02670248613</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>263.5178140444795</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>117.743157738966</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>634.7842078666346</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>1.751105455438916</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>9.943593194490346</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>1.260719159531667</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>2.366651336923406</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>0.06476768967898497</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>0.5467173852690022</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -17958,6 +18374,45 @@
       <c r="AC11" t="n">
         <v>0.5650012467231937</v>
       </c>
+      <c r="AD11" t="n">
+        <v>3.046629639623478</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>16.64908950634315</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>2094.826259174193</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>259.3494141241315</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>117.6907726442314</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>649.5639378996601</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>1.731496794266508</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>10.01194091149132</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>1.247471202308046</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>2.40296040380903</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>0.06402635927685921</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>0.5622807149132506</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -18053,6 +18508,45 @@
       <c r="AC12" t="n">
         <v>0.5495166752198273</v>
       </c>
+      <c r="AD12" t="n">
+        <v>3.09183620704292</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>16.5280063047552</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>2072.321507831768</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH12" t="n">
+        <v>256.4397785578516</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>115.765407776385</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>637.9393877783244</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>1.705855095003441</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>9.615241265334641</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>1.223501563987967</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>2.324303818865154</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>0.06149672497613987</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>0.5468063068008432</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -18148,6 +18642,45 @@
       <c r="AC13" t="n">
         <v>0.5502316495184391</v>
       </c>
+      <c r="AD13" t="n">
+        <v>2.918147954323878</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>16.55951045181903</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>2063.619148670997</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>252.8991996404884</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>115.0606967095611</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>636.8135504047822</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>1.70576258909959</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>9.613184642496599</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>1.203894745678302</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>2.320344468880381</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>0.06376360560949154</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0.5475257201749377</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -18243,6 +18776,45 @@
       <c r="AC14" t="n">
         <v>0.5434953026934386</v>
       </c>
+      <c r="AD14" t="n">
+        <v>3.032487225675411</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>16.57773245808293</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>2094.898218771554</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>256.7819666282213</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>115.1270727154248</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>636.1880011823118</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>1.711796496873089</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>9.774159185210252</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>1.239114440998222</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>2.337339248418536</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>0.06410797353251561</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>0.5408148035940263</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -18338,6 +18910,45 @@
       <c r="AC15" t="n">
         <v>0.5698229062407644</v>
       </c>
+      <c r="AD15" t="n">
+        <v>3.039162168810725</v>
+      </c>
+      <c r="AE15" t="n">
+        <v>16.82476522708093</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>2098.806643751228</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>262.2327374344755</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>117.5501353414752</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>640.8145630682449</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>1.724338443176569</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>9.838238856610698</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>1.235049547893554</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>2.369862172697205</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>0.06421886627730329</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>0.5670101405872291</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -18433,6 +19044,45 @@
       <c r="AC16" t="n">
         <v>0.5584054757670992</v>
       </c>
+      <c r="AD16" t="n">
+        <v>3.025582583608641</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>16.58399698824823</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>2103.117262912997</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>3674.908202193714</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>260.613542070295</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>117.4814281507359</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>648.9045468743706</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>1.748466226787774</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>9.821386536201379</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>1.246916263363856</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>2.346920434288331</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>0.06297142613950102</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>0.5556463567538458</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -18528,6 +19178,45 @@
       <c r="AC17" t="n">
         <v>0.2735683335858453</v>
       </c>
+      <c r="AD17" t="n">
+        <v>0.508084154725893</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>1235.369257783203</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>2253.44286697373</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>2396.46791492262</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>1703.522737698909</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>1183.715815321626</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>2329.623738488579</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>7.843558247071055</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>2.622982263003141</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>0.3284105450456155</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>0.9150412117090377</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>0.04784663774684041</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>0.2735427007428565</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -18623,6 +19312,45 @@
       <c r="AC18" t="n">
         <v>0.1703618690694655</v>
       </c>
+      <c r="AD18" t="n">
+        <v>0.4725483187810663</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>1174.388264012084</v>
+      </c>
+      <c r="AF18" t="n">
+        <v>2168.893470484474</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>2396.46791492262</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>1555.091187918796</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>1171.526610699623</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>2218.765582911176</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>6.796286281190197</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>2.294313885891203</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>0.3167975100674</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>0.7065289525394467</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>0.04458361158018932</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>0.1703226554681902</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -18718,6 +19446,45 @@
       <c r="AC19" t="n">
         <v>0.1750879373994345</v>
       </c>
+      <c r="AD19" t="n">
+        <v>0.5079593006682761</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>1172.645024000954</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>2138.281429832199</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>2396.46791492262</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>1578.162055610088</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>1170.009785775367</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>2170.060361814114</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>6.771353143318334</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>2.214317436956726</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>0.3148940126746722</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>0.6821872197197784</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>0.05072212141196186</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>0.1750474850448548</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -18813,6 +19580,45 @@
       <c r="AC20" t="n">
         <v>0.1769138997101105</v>
       </c>
+      <c r="AD20" t="n">
+        <v>0.4484950687012397</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>1175.054907599417</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>2165.464204759148</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>2396.46791492262</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>1564.625688904452</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>1182.655011026648</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>2174.690461340442</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>6.822448692262152</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>2.302126417414333</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>0.3256615067701371</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>0.6923830389446824</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>0.04547196461374302</v>
+      </c>
+      <c r="AP20" t="n">
+        <v>0.1768769853161549</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -18907,6 +19713,45 @@
       </c>
       <c r="AC21" t="n">
         <v>0.1764563978547965</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0.4863679133968036</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>1167.655682181899</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>2137.103638180532</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>2396.46791492262</v>
+      </c>
+      <c r="AH21" t="n">
+        <v>1552.332892806679</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>1166.432074468111</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>2153.519990963594</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>6.657416559780061</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>2.200279969070592</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>0.3077340504157632</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>0.672547099055717</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>0.04887524849853255</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>0.1764156061081543</v>
       </c>
     </row>
   </sheetData>
@@ -20141,7 +20986,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC6"/>
+  <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20232,67 +21077,132 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>7Li_se</t>
+          <t>7Li_exterr</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>24Mg_se</t>
+          <t>24Mg_exterr</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>27Al_se</t>
+          <t>27Al_exterr</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>29Si_se</t>
+          <t>29Si_exterr</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>43Ca_se</t>
+          <t>43Ca_exterr</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>48Ti_se</t>
+          <t>48Ti_exterr</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>57Fe_se</t>
+          <t>57Fe_exterr</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>88Sr_se</t>
+          <t>88Sr_exterr</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>138Ba_se</t>
+          <t>138Ba_exterr</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>139La_se</t>
+          <t>139La_exterr</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>140Ce_se</t>
+          <t>140Ce_exterr</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>153Eu_se</t>
+          <t>153Eu_exterr</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>208Pb_se</t>
+          <t>208Pb_exterr</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>7Li_interr</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>24Mg_interr</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>27Al_interr</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>29Si_interr</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>43Ca_interr</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>48Ti_interr</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>57Fe_interr</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>88Sr_interr</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>138Ba_interr</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>139La_interr</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>140Ce_interr</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>153Eu_interr</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>208Pb_interr</t>
         </is>
       </c>
     </row>
@@ -20390,6 +21300,45 @@
       <c r="AC2" t="n">
         <v>3.63511914452108</v>
       </c>
+      <c r="AD2" t="n">
+        <v>4.310849861348289</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>5.79278467072074</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>349.4331594922516</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>3494.8440318784</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>1814.18137754411</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>33.51772433195656</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>4.133081606343394</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>1.515862785444546</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.7340012681887673</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.8637873930834047</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.7748579719358629</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.7405824009823327</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>3.614033336049892</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -20485,6 +21434,45 @@
       <c r="AC3" t="n">
         <v>3.590855959057254</v>
       </c>
+      <c r="AD3" t="n">
+        <v>4.384640618949425</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>3.848289933397186</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>347.9949171628779</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>3494.8440318784</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>1813.954037752538</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>33.43110354783111</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>2.082937594836802</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1.520716260653602</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0.7244540637823822</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.8503511317123591</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.7726704324317801</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.7468615396971675</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>3.570031963930742</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -20580,6 +21568,45 @@
       <c r="AC4" t="n">
         <v>3.695273597792309</v>
       </c>
+      <c r="AD4" t="n">
+        <v>4.420436030378218</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>1.93363599248161</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>351.6339565545468</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>3494.8440318784</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>1860.901541509482</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>34.80585753270905</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>2.306940926423347</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>1.563118915501478</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>0.7588899557159853</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>0.8892015069739104</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>0.7969731978764486</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0.7664447516724296</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>3.673819316244001</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -20675,6 +21702,45 @@
       <c r="AC5" t="n">
         <v>3.687379287968199</v>
       </c>
+      <c r="AD5" t="n">
+        <v>4.167334823323447</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1.928058216505245</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>355.8415374699192</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>3494.8440318784</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>1848.860454885024</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>34.43261770125828</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>2.583524431629171</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>1.550515326003251</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0.7597187995662145</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0.8729114067304686</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0.7836380924989667</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.7671728752419564</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>3.66597850093768</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -20769,6 +21835,45 @@
       </c>
       <c r="AC6" t="n">
         <v>3.660260050526333</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>4.177660414211473</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>1.943673197241472</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>351.2263165169414</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>3494.8440318784</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>1828.035083032504</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>34.21461636363728</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>1.966109823816679</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>1.533575607467014</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.7385365934077393</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.8468605764498519</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.7651156832965907</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.7543417654773046</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>3.639020558077191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorg to submodules 0.1.0
</commit_message>
<xml_diff>
--- a/test_data/lasercalc_example_export_BCR-2G.xlsx
+++ b/test_data/lasercalc_example_export_BCR-2G.xlsx
@@ -6012,7 +6012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EU18"/>
+  <dimension ref="A1:EU19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10957,7 +10957,7 @@
         <v>120</v>
       </c>
       <c r="DB11" t="n">
-        <v>0</v>
+        <v>0.174</v>
       </c>
       <c r="DC11" t="n">
         <v>0.17</v>
@@ -14133,6 +14133,417 @@
       <c r="EU18" t="n">
         <v>180</v>
       </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>NIST-616</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="G19" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.0292</v>
+      </c>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0.0173</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.0157</v>
+      </c>
+      <c r="U19" t="n">
+        <v>0.0146</v>
+      </c>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="n">
+        <v>16</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.0162</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0.283</v>
+      </c>
+      <c r="AA19" t="n">
+        <v>0.0154</v>
+      </c>
+      <c r="AB19" t="n">
+        <v>0.0169</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>0.0302</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>0.0298</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>0.895</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>0.0145</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>0.609</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>0.08790000000000001</v>
+      </c>
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="n">
+        <v>0.0194</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>0.0227</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>0.435</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>13</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0.0036</v>
+      </c>
+      <c r="AT19" t="inlineStr"/>
+      <c r="AU19" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="AV19" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="AW19" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="AX19" t="n">
+        <v>338891.61659704</v>
+      </c>
+      <c r="AY19" t="n">
+        <v>0.0164</v>
+      </c>
+      <c r="AZ19" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="BA19" t="n">
+        <v>41.72</v>
+      </c>
+      <c r="BB19" t="n">
+        <v>0.0299</v>
+      </c>
+      <c r="BC19" t="n">
+        <v>0.0145</v>
+      </c>
+      <c r="BD19" t="n">
+        <v>0.0252</v>
+      </c>
+      <c r="BE19" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="BF19" t="n">
+        <v>0.0081</v>
+      </c>
+      <c r="BG19" t="n">
+        <v>0.0144</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>0.0721</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="BJ19" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="BK19" t="n">
+        <v>0.0288</v>
+      </c>
+      <c r="BL19" t="n">
+        <v>0.0171</v>
+      </c>
+      <c r="BM19" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="BN19" t="n">
+        <v>0.0951</v>
+      </c>
+      <c r="BO19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BP19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR19" t="n">
+        <v>0.012</v>
+      </c>
+      <c r="BS19" t="n">
+        <v>0.235</v>
+      </c>
+      <c r="BT19" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="BU19" t="n">
+        <v>0.0125</v>
+      </c>
+      <c r="BV19" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="BW19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BY19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ19" t="n">
+        <v>0.00055</v>
+      </c>
+      <c r="CA19" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB19" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="CC19" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="CD19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="CE19" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="CF19" t="n">
+        <v>0.0007</v>
+      </c>
+      <c r="CG19" t="n">
+        <v>0.00065</v>
+      </c>
+      <c r="CH19" t="n">
+        <v>0.00035</v>
+      </c>
+      <c r="CI19" t="n">
+        <v>0</v>
+      </c>
+      <c r="CJ19" t="n">
+        <v>4</v>
+      </c>
+      <c r="CK19" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="CL19" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="CM19" t="n">
+        <v>0.0195</v>
+      </c>
+      <c r="CN19" t="n">
+        <v>0.0009</v>
+      </c>
+      <c r="CO19" t="n">
+        <v>0.00155</v>
+      </c>
+      <c r="CP19" t="n">
+        <v>0.00175</v>
+      </c>
+      <c r="CQ19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="CR19" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="CS19" t="n">
+        <v>0.0295</v>
+      </c>
+      <c r="CT19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="CU19" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="CV19" t="n">
+        <v>0.0135</v>
+      </c>
+      <c r="CW19" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="CX19" t="n">
+        <v>0</v>
+      </c>
+      <c r="CY19" t="n">
+        <v>0.00075</v>
+      </c>
+      <c r="CZ19" t="n">
+        <v>0.00155</v>
+      </c>
+      <c r="DA19" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="DB19" t="n">
+        <v>5</v>
+      </c>
+      <c r="DC19" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="DD19" t="n">
+        <v>0.00045</v>
+      </c>
+      <c r="DE19" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="DF19" t="n">
+        <v>0.00065</v>
+      </c>
+      <c r="DG19" t="n">
+        <v>0</v>
+      </c>
+      <c r="DH19" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="DI19" t="n">
+        <v>0</v>
+      </c>
+      <c r="DJ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="DK19" t="n">
+        <v>3272.056</v>
+      </c>
+      <c r="DL19" t="n">
+        <v>0.00145</v>
+      </c>
+      <c r="DM19" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="DN19" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="DO19" t="n">
+        <v>0.00275</v>
+      </c>
+      <c r="DP19" t="n">
+        <v>0.00105</v>
+      </c>
+      <c r="DQ19" t="n">
+        <v>0.0035</v>
+      </c>
+      <c r="DR19" t="n">
+        <v>0.145</v>
+      </c>
+      <c r="DS19" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="DT19" t="n">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="DU19" t="n">
+        <v>0.00065</v>
+      </c>
+      <c r="DV19" t="n">
+        <v>0.0075</v>
+      </c>
+      <c r="DW19" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="DX19" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="DY19" t="n">
+        <v>0.00115</v>
+      </c>
+      <c r="DZ19" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="EA19" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="EB19" t="n">
+        <v>725000</v>
+      </c>
+      <c r="EC19" t="inlineStr"/>
+      <c r="ED19" t="inlineStr"/>
+      <c r="EE19" t="inlineStr"/>
+      <c r="EF19" t="inlineStr"/>
+      <c r="EG19" t="inlineStr"/>
+      <c r="EH19" t="inlineStr"/>
+      <c r="EI19" t="n">
+        <v>13700</v>
+      </c>
+      <c r="EJ19" t="inlineStr"/>
+      <c r="EK19" t="inlineStr"/>
+      <c r="EL19" t="n">
+        <v>7000</v>
+      </c>
+      <c r="EM19" t="inlineStr"/>
+      <c r="EN19" t="inlineStr"/>
+      <c r="EO19" t="inlineStr"/>
+      <c r="EP19" t="inlineStr"/>
+      <c r="EQ19" t="inlineStr"/>
+      <c r="ER19" t="inlineStr"/>
+      <c r="ES19" t="n">
+        <v>9000</v>
+      </c>
+      <c r="ET19" t="inlineStr"/>
+      <c r="EU19" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -16348,7 +16759,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.0004499628318596198</v>
+        <v>0.00044996283185962</v>
       </c>
       <c r="D2" t="n">
         <v>21.67426632758452</v>
@@ -16504,7 +16915,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.190534078267105e-07</v>
+        <v>2.190534078267104e-07</v>
       </c>
       <c r="D6" t="n">
         <v>96.6589318091596</v>
@@ -16660,7 +17071,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2.073748466128361e-10</v>
+        <v>2.07374846612836e-10</v>
       </c>
       <c r="D10" t="n">
         <v>305.2878357762683</v>
@@ -16699,7 +17110,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>7.243159635597474e-09</v>
+        <v>7.243159635597471e-09</v>
       </c>
       <c r="D11" t="n">
         <v>171.6331609126637</v>
@@ -16738,7 +17149,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>9.203588038047527e-10</v>
+        <v>9.203588038047518e-10</v>
       </c>
       <c r="D12" t="n">
         <v>240.2603930248168</v>
@@ -16777,7 +17188,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4.030016928614415e-09</v>
+        <v>4.030016928614411e-09</v>
       </c>
       <c r="D13" t="n">
         <v>188.9742400927013</v>
@@ -16816,7 +17227,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5.322208261827458e-09</v>
+        <v>5.322208261827455e-09</v>
       </c>
       <c r="D14" t="n">
         <v>180.5529546364902</v>
@@ -17169,43 +17580,43 @@
         <v>0.6644538762439895</v>
       </c>
       <c r="AD2" t="n">
-        <v>2.99884954517325</v>
+        <v>0.8252859321763683</v>
       </c>
       <c r="AE2" t="n">
-        <v>48.89894113114184</v>
+        <v>46.75956669775771</v>
       </c>
       <c r="AF2" t="n">
-        <v>2054.470196328495</v>
+        <v>696.1073497143615</v>
       </c>
       <c r="AG2" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH2" t="n">
-        <v>288.3988600395895</v>
+        <v>225.2351453019907</v>
       </c>
       <c r="AI2" t="n">
-        <v>111.107842412584</v>
+        <v>24.33602386331645</v>
       </c>
       <c r="AJ2" t="n">
-        <v>611.0676505325631</v>
+        <v>249.3313075740208</v>
       </c>
       <c r="AK2" t="n">
-        <v>1.687864375368129</v>
+        <v>1.367797867563141</v>
       </c>
       <c r="AL2" t="n">
-        <v>9.692056101501699</v>
+        <v>8.46077143018371</v>
       </c>
       <c r="AM2" t="n">
-        <v>1.221923406170256</v>
+        <v>1.046962491145324</v>
       </c>
       <c r="AN2" t="n">
-        <v>2.317004528629859</v>
+        <v>2.123920204474599</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.0648134729050522</v>
+        <v>0.06039825921122582</v>
       </c>
       <c r="AP2" t="n">
-        <v>0.6622267791898836</v>
+        <v>0.3934685797029261</v>
       </c>
     </row>
     <row r="3">
@@ -17303,43 +17714,43 @@
         <v>0.5331471995062036</v>
       </c>
       <c r="AD3" t="n">
-        <v>3.063484187314715</v>
+        <v>0.8351237351021986</v>
       </c>
       <c r="AE3" t="n">
-        <v>15.96768893768607</v>
+        <v>7.298287030641506</v>
       </c>
       <c r="AF3" t="n">
-        <v>2052.029463518423</v>
+        <v>680.6291417736679</v>
       </c>
       <c r="AG3" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH3" t="n">
-        <v>255.7431783670662</v>
+        <v>183.5297894218344</v>
       </c>
       <c r="AI3" t="n">
-        <v>112.5062105657118</v>
+        <v>24.24242561597299</v>
       </c>
       <c r="AJ3" t="n">
-        <v>611.8986831716545</v>
+        <v>241.4650496039297</v>
       </c>
       <c r="AK3" t="n">
-        <v>1.683607805334793</v>
+        <v>1.35618237037631</v>
       </c>
       <c r="AL3" t="n">
-        <v>9.458524230717785</v>
+        <v>8.200378584561971</v>
       </c>
       <c r="AM3" t="n">
-        <v>1.201585809031792</v>
+        <v>1.02747411275684</v>
       </c>
       <c r="AN3" t="n">
-        <v>2.279990595576796</v>
+        <v>2.082203187846552</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.06154961528371558</v>
+        <v>0.05668393757181263</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.5305181401048905</v>
+        <v>0.1136438641040705</v>
       </c>
     </row>
     <row r="4">
@@ -17437,43 +17848,43 @@
         <v>0.5566525763285903</v>
       </c>
       <c r="AD4" t="n">
-        <v>3.013958139085485</v>
+        <v>0.8219493157803187</v>
       </c>
       <c r="AE4" t="n">
-        <v>17.16654268608011</v>
+        <v>8.974538962074005</v>
       </c>
       <c r="AF4" t="n">
-        <v>2081.344579068213</v>
+        <v>710.7809621043049</v>
       </c>
       <c r="AG4" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH4" t="n">
-        <v>260.5078612846243</v>
+        <v>183.7050650698579</v>
       </c>
       <c r="AI4" t="n">
-        <v>115.0057949850195</v>
+        <v>25.00493755951468</v>
       </c>
       <c r="AJ4" t="n">
-        <v>625.0929332459941</v>
+        <v>250.6649390840211</v>
       </c>
       <c r="AK4" t="n">
-        <v>1.737508862968636</v>
+        <v>1.401475327380453</v>
       </c>
       <c r="AL4" t="n">
-        <v>9.851096965883187</v>
+        <v>8.575375183937382</v>
       </c>
       <c r="AM4" t="n">
-        <v>1.256847508806852</v>
+        <v>1.076299359811143</v>
       </c>
       <c r="AN4" t="n">
-        <v>2.372410924149129</v>
+        <v>2.169499274250827</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.06488106396811474</v>
+        <v>0.06012411246738152</v>
       </c>
       <c r="AP4" t="n">
-        <v>0.5540364298939671</v>
+        <v>0.1671148759976118</v>
       </c>
     </row>
     <row r="5">
@@ -17571,43 +17982,43 @@
         <v>0.5448124450633746</v>
       </c>
       <c r="AD5" t="n">
-        <v>3.051264093685064</v>
+        <v>0.8312164390169015</v>
       </c>
       <c r="AE5" t="n">
-        <v>16.41450068572062</v>
+        <v>7.638625613271928</v>
       </c>
       <c r="AF5" t="n">
-        <v>2071.437042740539</v>
+        <v>691.3425794071833</v>
       </c>
       <c r="AG5" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH5" t="n">
-        <v>263.2575557525885</v>
+        <v>192.6848008492933</v>
       </c>
       <c r="AI5" t="n">
-        <v>114.6491165379979</v>
+        <v>24.79986708058141</v>
       </c>
       <c r="AJ5" t="n">
-        <v>627.9086184498912</v>
+        <v>250.2643226578481</v>
       </c>
       <c r="AK5" t="n">
-        <v>1.724226175882502</v>
+        <v>1.388707164164284</v>
       </c>
       <c r="AL5" t="n">
-        <v>9.815957466681054</v>
+        <v>8.516130048005699</v>
       </c>
       <c r="AM5" t="n">
-        <v>1.245431961277169</v>
+        <v>1.066695032786934</v>
       </c>
       <c r="AN5" t="n">
-        <v>2.338513401763503</v>
+        <v>2.136676518204002</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.0639069417626261</v>
+        <v>0.05896929170858412</v>
       </c>
       <c r="AP5" t="n">
-        <v>0.5421317640714155</v>
+        <v>0.1187736889375374</v>
       </c>
     </row>
     <row r="6">
@@ -17705,43 +18116,43 @@
         <v>0.5678599065224346</v>
       </c>
       <c r="AD6" t="n">
-        <v>3.097347602283943</v>
+        <v>0.8484204417478058</v>
       </c>
       <c r="AE6" t="n">
-        <v>16.72955856561553</v>
+        <v>7.724596329402087</v>
       </c>
       <c r="AF6" t="n">
-        <v>2094.771179519221</v>
+        <v>701.7579161524087</v>
       </c>
       <c r="AG6" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH6" t="n">
-        <v>266.1213050856113</v>
+        <v>191.0794203270988</v>
       </c>
       <c r="AI6" t="n">
-        <v>116.7266881221813</v>
+        <v>25.48872641194832</v>
       </c>
       <c r="AJ6" t="n">
-        <v>628.3835748407728</v>
+        <v>251.551553437094</v>
       </c>
       <c r="AK6" t="n">
-        <v>1.748732673360951</v>
+        <v>1.408674818160468</v>
       </c>
       <c r="AL6" t="n">
-        <v>10.00092050331233</v>
+        <v>8.688869447119107</v>
       </c>
       <c r="AM6" t="n">
-        <v>1.261438857762394</v>
+        <v>1.079198296534234</v>
       </c>
       <c r="AN6" t="n">
-        <v>2.390571890564169</v>
+        <v>2.185768017747785</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.06643033124233753</v>
+        <v>0.06166788768973908</v>
       </c>
       <c r="AP6" t="n">
-        <v>0.5650628078403056</v>
+        <v>0.1224554420388375</v>
       </c>
     </row>
     <row r="7">
@@ -17839,43 +18250,43 @@
         <v>0.5662956448359023</v>
       </c>
       <c r="AD7" t="n">
-        <v>3.148340124627654</v>
+        <v>0.8619064695955538</v>
       </c>
       <c r="AE7" t="n">
-        <v>16.61207386922101</v>
+        <v>7.625756058302615</v>
       </c>
       <c r="AF7" t="n">
-        <v>2079.084315315049</v>
+        <v>694.7355618615439</v>
       </c>
       <c r="AG7" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH7" t="n">
-        <v>267.5037539872917</v>
+        <v>195.595789086088</v>
       </c>
       <c r="AI7" t="n">
-        <v>116.6716110198576</v>
+        <v>25.31569698960931</v>
       </c>
       <c r="AJ7" t="n">
-        <v>637.1359167474503</v>
+        <v>254.8418898767785</v>
       </c>
       <c r="AK7" t="n">
-        <v>1.752277281380337</v>
+        <v>1.417236342191466</v>
       </c>
       <c r="AL7" t="n">
-        <v>9.983931239484622</v>
+        <v>8.687227475848905</v>
       </c>
       <c r="AM7" t="n">
-        <v>1.257580190222183</v>
+        <v>1.075779827889936</v>
       </c>
       <c r="AN7" t="n">
-        <v>2.412926728357637</v>
+        <v>2.208137037534713</v>
       </c>
       <c r="AO7" t="n">
-        <v>0.0668838391239651</v>
+        <v>0.06210976184750645</v>
       </c>
       <c r="AP7" t="n">
-        <v>0.5635078113309172</v>
+        <v>0.1228146392161332</v>
       </c>
     </row>
     <row r="8">
@@ -17973,43 +18384,43 @@
         <v>0.5625624787611712</v>
       </c>
       <c r="AD8" t="n">
-        <v>3.159637294009065</v>
+        <v>0.8544907540747751</v>
       </c>
       <c r="AE8" t="n">
-        <v>16.85472657989437</v>
+        <v>7.883058629382739</v>
       </c>
       <c r="AF8" t="n">
-        <v>2112.818711005713</v>
+        <v>723.3653819732699</v>
       </c>
       <c r="AG8" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH8" t="n">
-        <v>267.0079023070129</v>
+        <v>191.5429627734972</v>
       </c>
       <c r="AI8" t="n">
-        <v>118.4358305629869</v>
+        <v>26.07430446584228</v>
       </c>
       <c r="AJ8" t="n">
-        <v>641.1284596286813</v>
+        <v>259.9569236205006</v>
       </c>
       <c r="AK8" t="n">
-        <v>1.795034333221278</v>
+        <v>1.457183763356519</v>
       </c>
       <c r="AL8" t="n">
-        <v>10.17228462369724</v>
+        <v>8.868936337171819</v>
       </c>
       <c r="AM8" t="n">
-        <v>1.281551318539665</v>
+        <v>1.10118127111554</v>
       </c>
       <c r="AN8" t="n">
-        <v>2.445148069826108</v>
+        <v>2.239732124246355</v>
       </c>
       <c r="AO8" t="n">
-        <v>0.06414456886466371</v>
+        <v>0.05901458447722477</v>
       </c>
       <c r="AP8" t="n">
-        <v>0.5597793824161401</v>
+        <v>0.1157731349843886</v>
       </c>
     </row>
     <row r="9">
@@ -18107,43 +18518,43 @@
         <v>0.5622388184462893</v>
       </c>
       <c r="AD9" t="n">
-        <v>3.086683972577208</v>
+        <v>0.8383124391757713</v>
       </c>
       <c r="AE9" t="n">
-        <v>16.69125305716587</v>
+        <v>7.902295030791174</v>
       </c>
       <c r="AF9" t="n">
-        <v>2087.533201793496</v>
+        <v>706.4142462921204</v>
       </c>
       <c r="AG9" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH9" t="n">
-        <v>263.6378708495386</v>
+        <v>189.5445005008482</v>
       </c>
       <c r="AI9" t="n">
-        <v>118.3240095599956</v>
+        <v>25.95591351381763</v>
       </c>
       <c r="AJ9" t="n">
-        <v>638.0907190648031</v>
+        <v>255.8011446572502</v>
       </c>
       <c r="AK9" t="n">
-        <v>1.76300325192444</v>
+        <v>1.4262278300397</v>
       </c>
       <c r="AL9" t="n">
-        <v>10.0136251965347</v>
+        <v>8.716275721474517</v>
       </c>
       <c r="AM9" t="n">
-        <v>1.262837401112847</v>
+        <v>1.079167560525672</v>
       </c>
       <c r="AN9" t="n">
-        <v>2.42992066217099</v>
+        <v>2.224418241399063</v>
       </c>
       <c r="AO9" t="n">
-        <v>0.06487385524833321</v>
+        <v>0.05986973808332359</v>
       </c>
       <c r="AP9" t="n">
-        <v>0.5594649593380577</v>
+        <v>0.1192351207550541</v>
       </c>
     </row>
     <row r="10">
@@ -18241,43 +18652,43 @@
         <v>0.549423481163317</v>
       </c>
       <c r="AD10" t="n">
-        <v>3.112864385663483</v>
+        <v>0.8529582714271625</v>
       </c>
       <c r="AE10" t="n">
-        <v>16.67851658484326</v>
+        <v>7.691462612758346</v>
       </c>
       <c r="AF10" t="n">
-        <v>2086.02670248613</v>
+        <v>701.8195904947427</v>
       </c>
       <c r="AG10" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH10" t="n">
-        <v>263.5178140444795</v>
+        <v>189.3999172696874</v>
       </c>
       <c r="AI10" t="n">
-        <v>117.743157738966</v>
+        <v>25.62866163781824</v>
       </c>
       <c r="AJ10" t="n">
-        <v>634.7842078666346</v>
+        <v>253.9669665221831</v>
       </c>
       <c r="AK10" t="n">
-        <v>1.751105455438916</v>
+        <v>1.415092335367673</v>
       </c>
       <c r="AL10" t="n">
-        <v>9.943593194490346</v>
+        <v>8.65626575829226</v>
       </c>
       <c r="AM10" t="n">
-        <v>1.260719159531667</v>
+        <v>1.079122451120266</v>
       </c>
       <c r="AN10" t="n">
-        <v>2.366651336923406</v>
+        <v>2.161986831302537</v>
       </c>
       <c r="AO10" t="n">
-        <v>0.06476768967898497</v>
+        <v>0.06018682450649736</v>
       </c>
       <c r="AP10" t="n">
-        <v>0.5467173852690022</v>
+        <v>0.1185651263308148</v>
       </c>
     </row>
     <row r="11">
@@ -18375,43 +18786,43 @@
         <v>0.5650012467231937</v>
       </c>
       <c r="AD11" t="n">
-        <v>3.046629639623478</v>
+        <v>0.8331710350772541</v>
       </c>
       <c r="AE11" t="n">
-        <v>16.64908950634315</v>
+        <v>7.740884806185411</v>
       </c>
       <c r="AF11" t="n">
-        <v>2094.826259174193</v>
+        <v>708.5419376978625</v>
       </c>
       <c r="AG11" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH11" t="n">
-        <v>259.3494141241315</v>
+        <v>183.7268220012597</v>
       </c>
       <c r="AI11" t="n">
-        <v>117.6907726442314</v>
+        <v>25.71736472480174</v>
       </c>
       <c r="AJ11" t="n">
-        <v>649.5639378996601</v>
+        <v>261.9601181949556</v>
       </c>
       <c r="AK11" t="n">
-        <v>1.731496794266508</v>
+        <v>1.397877047688177</v>
       </c>
       <c r="AL11" t="n">
-        <v>10.01194091149132</v>
+        <v>8.723604702649371</v>
       </c>
       <c r="AM11" t="n">
-        <v>1.247471202308046</v>
+        <v>1.068432222589955</v>
       </c>
       <c r="AN11" t="n">
-        <v>2.40296040380903</v>
+        <v>2.201660653584014</v>
       </c>
       <c r="AO11" t="n">
-        <v>0.06402635927685921</v>
+        <v>0.05915966183727141</v>
       </c>
       <c r="AP11" t="n">
-        <v>0.5622807149132506</v>
+        <v>0.1471815492942153</v>
       </c>
     </row>
     <row r="12">
@@ -18509,43 +18920,43 @@
         <v>0.5495166752198273</v>
       </c>
       <c r="AD12" t="n">
-        <v>3.09183620704292</v>
+        <v>0.834240899061065</v>
       </c>
       <c r="AE12" t="n">
-        <v>16.5280063047552</v>
+        <v>7.686159793759878</v>
       </c>
       <c r="AF12" t="n">
-        <v>2072.321507831768</v>
+        <v>701.8376043350511</v>
       </c>
       <c r="AG12" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH12" t="n">
-        <v>256.4397785578516</v>
+        <v>187.3371555127301</v>
       </c>
       <c r="AI12" t="n">
-        <v>115.765407776385</v>
+        <v>25.13846952243929</v>
       </c>
       <c r="AJ12" t="n">
-        <v>637.9393877783244</v>
+        <v>253.3537229229596</v>
       </c>
       <c r="AK12" t="n">
-        <v>1.705855095003441</v>
+        <v>1.380006088824754</v>
       </c>
       <c r="AL12" t="n">
-        <v>9.615241265334641</v>
+        <v>8.378990194840116</v>
       </c>
       <c r="AM12" t="n">
-        <v>1.223501563987967</v>
+        <v>1.048437132777449</v>
       </c>
       <c r="AN12" t="n">
-        <v>2.324303818865154</v>
+        <v>2.128628660821677</v>
       </c>
       <c r="AO12" t="n">
-        <v>0.06149672497613987</v>
+        <v>0.0566581855632144</v>
       </c>
       <c r="AP12" t="n">
-        <v>0.5468063068008432</v>
+        <v>0.1168666085758115</v>
       </c>
     </row>
     <row r="13">
@@ -18643,43 +19054,43 @@
         <v>0.5502316495184391</v>
       </c>
       <c r="AD13" t="n">
-        <v>2.918147954323878</v>
+        <v>0.8097055146021254</v>
       </c>
       <c r="AE13" t="n">
-        <v>16.55951045181903</v>
+        <v>7.653322835548636</v>
       </c>
       <c r="AF13" t="n">
-        <v>2063.619148670997</v>
+        <v>697.6702691000255</v>
       </c>
       <c r="AG13" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH13" t="n">
-        <v>252.8991996404884</v>
+        <v>178.7407348817541</v>
       </c>
       <c r="AI13" t="n">
-        <v>115.0606967095611</v>
+        <v>25.15503008084625</v>
       </c>
       <c r="AJ13" t="n">
-        <v>636.8135504047822</v>
+        <v>259.8289714497894</v>
       </c>
       <c r="AK13" t="n">
-        <v>1.70576258909959</v>
+        <v>1.382322722140557</v>
       </c>
       <c r="AL13" t="n">
-        <v>9.613184642496599</v>
+        <v>8.355573950121263</v>
       </c>
       <c r="AM13" t="n">
-        <v>1.203894745678302</v>
+        <v>1.031162295708442</v>
       </c>
       <c r="AN13" t="n">
-        <v>2.320344468880381</v>
+        <v>2.124609399665712</v>
       </c>
       <c r="AO13" t="n">
-        <v>0.06376360560949154</v>
+        <v>0.05921293138194621</v>
       </c>
       <c r="AP13" t="n">
-        <v>0.5475257201749377</v>
+        <v>0.1205806694883212</v>
       </c>
     </row>
     <row r="14">
@@ -18777,43 +19188,43 @@
         <v>0.5434953026934386</v>
       </c>
       <c r="AD14" t="n">
-        <v>3.032487225675411</v>
+        <v>0.8256240569649598</v>
       </c>
       <c r="AE14" t="n">
-        <v>16.57773245808293</v>
+        <v>7.714802619514612</v>
       </c>
       <c r="AF14" t="n">
-        <v>2094.898218771554</v>
+        <v>709.0397244071912</v>
       </c>
       <c r="AG14" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH14" t="n">
-        <v>256.7819666282213</v>
+        <v>184.9692782825286</v>
       </c>
       <c r="AI14" t="n">
-        <v>115.1270727154248</v>
+        <v>25.16236960099299</v>
       </c>
       <c r="AJ14" t="n">
-        <v>636.1880011823118</v>
+        <v>257.6233323212759</v>
       </c>
       <c r="AK14" t="n">
-        <v>1.711796496873089</v>
+        <v>1.386390779545268</v>
       </c>
       <c r="AL14" t="n">
-        <v>9.774159185210252</v>
+        <v>8.513229584400557</v>
       </c>
       <c r="AM14" t="n">
-        <v>1.239114440998222</v>
+        <v>1.06221868517904</v>
       </c>
       <c r="AN14" t="n">
-        <v>2.337339248418536</v>
+        <v>2.137341032416392</v>
       </c>
       <c r="AO14" t="n">
-        <v>0.06410797353251561</v>
+        <v>0.05925261441648563</v>
       </c>
       <c r="AP14" t="n">
-        <v>0.5408148035940263</v>
+        <v>0.1156632945244958</v>
       </c>
     </row>
     <row r="15">
@@ -18911,43 +19322,43 @@
         <v>0.5698229062407644</v>
       </c>
       <c r="AD15" t="n">
-        <v>3.039162168810725</v>
+        <v>0.8257877170836112</v>
       </c>
       <c r="AE15" t="n">
-        <v>16.82476522708093</v>
+        <v>7.771525725640419</v>
       </c>
       <c r="AF15" t="n">
-        <v>2098.806643751228</v>
+        <v>703.4758080652732</v>
       </c>
       <c r="AG15" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH15" t="n">
-        <v>262.2327374344755</v>
+        <v>191.1939015524269</v>
       </c>
       <c r="AI15" t="n">
-        <v>117.5501353414752</v>
+        <v>25.61547581748122</v>
       </c>
       <c r="AJ15" t="n">
-        <v>640.8145630682449</v>
+        <v>257.143445299015</v>
       </c>
       <c r="AK15" t="n">
-        <v>1.724338443176569</v>
+        <v>1.390990395225364</v>
       </c>
       <c r="AL15" t="n">
-        <v>9.838238856610698</v>
+        <v>8.557066573129726</v>
       </c>
       <c r="AM15" t="n">
-        <v>1.235049547893554</v>
+        <v>1.057128079850119</v>
       </c>
       <c r="AN15" t="n">
-        <v>2.369862172697205</v>
+        <v>2.167440199805198</v>
       </c>
       <c r="AO15" t="n">
-        <v>0.06421886627730329</v>
+        <v>0.05956816348783518</v>
       </c>
       <c r="AP15" t="n">
-        <v>0.5670101405872291</v>
+        <v>0.1201633650251187</v>
       </c>
     </row>
     <row r="16">
@@ -19045,43 +19456,43 @@
         <v>0.5584054757670992</v>
       </c>
       <c r="AD16" t="n">
-        <v>3.025582583608641</v>
+        <v>0.82730434666178</v>
       </c>
       <c r="AE16" t="n">
-        <v>16.58399698824823</v>
+        <v>7.662447920256216</v>
       </c>
       <c r="AF16" t="n">
-        <v>2103.117262912997</v>
+        <v>704.7324126347049</v>
       </c>
       <c r="AG16" t="n">
-        <v>3674.908202193714</v>
+        <v>3272.251308900523</v>
       </c>
       <c r="AH16" t="n">
-        <v>260.613542070295</v>
+        <v>188.645008648944</v>
       </c>
       <c r="AI16" t="n">
-        <v>117.4814281507359</v>
+        <v>25.47104566765526</v>
       </c>
       <c r="AJ16" t="n">
-        <v>648.9045468743706</v>
+        <v>261.98228650609</v>
       </c>
       <c r="AK16" t="n">
-        <v>1.748466226787774</v>
+        <v>1.417824845976169</v>
       </c>
       <c r="AL16" t="n">
-        <v>9.821386536201379</v>
+        <v>8.538152662448654</v>
       </c>
       <c r="AM16" t="n">
-        <v>1.246916263363856</v>
+        <v>1.069875505418731</v>
       </c>
       <c r="AN16" t="n">
-        <v>2.346920434288331</v>
+        <v>2.144961768818006</v>
       </c>
       <c r="AO16" t="n">
-        <v>0.06297142613950102</v>
+        <v>0.05814104542954145</v>
       </c>
       <c r="AP16" t="n">
-        <v>0.5556463567538458</v>
+        <v>0.1165073116191062</v>
       </c>
     </row>
     <row r="17">
@@ -19179,43 +19590,43 @@
         <v>0.2735683335858453</v>
       </c>
       <c r="AD17" t="n">
-        <v>0.508084154725893</v>
+        <v>0.2335229131288413</v>
       </c>
       <c r="AE17" t="n">
-        <v>1235.369257783203</v>
+        <v>592.7727348732301</v>
       </c>
       <c r="AF17" t="n">
-        <v>2253.44286697373</v>
+        <v>767.6811502323878</v>
       </c>
       <c r="AG17" t="n">
-        <v>2396.46791492262</v>
+        <v>467.4644727000749</v>
       </c>
       <c r="AH17" t="n">
-        <v>1703.522737698909</v>
+        <v>1074.454362207458</v>
       </c>
       <c r="AI17" t="n">
-        <v>1183.715815321626</v>
+        <v>278.7122949309602</v>
       </c>
       <c r="AJ17" t="n">
-        <v>2329.623738488579</v>
+        <v>1073.198313181838</v>
       </c>
       <c r="AK17" t="n">
-        <v>7.843558247071055</v>
+        <v>5.885024557011827</v>
       </c>
       <c r="AL17" t="n">
-        <v>2.622982263003141</v>
+        <v>2.111759442633518</v>
       </c>
       <c r="AM17" t="n">
-        <v>0.3284105450456155</v>
+        <v>0.2566455959626625</v>
       </c>
       <c r="AN17" t="n">
-        <v>0.9150412117090377</v>
+        <v>0.815088303178916</v>
       </c>
       <c r="AO17" t="n">
-        <v>0.04784663774684041</v>
+        <v>0.04116756280893323</v>
       </c>
       <c r="AP17" t="n">
-        <v>0.2735427007428565</v>
+        <v>0.2156055340735251</v>
       </c>
     </row>
     <row r="18">
@@ -19313,43 +19724,43 @@
         <v>0.1703618690694655</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.4725483187810663</v>
+        <v>0.1550094563252535</v>
       </c>
       <c r="AE18" t="n">
-        <v>1174.388264012084</v>
+        <v>413.4976692768269</v>
       </c>
       <c r="AF18" t="n">
-        <v>2168.893470484474</v>
+        <v>468.0764253680608</v>
       </c>
       <c r="AG18" t="n">
-        <v>2396.46791492262</v>
+        <v>467.4644727000749</v>
       </c>
       <c r="AH18" t="n">
-        <v>1555.091187918796</v>
+        <v>833.9949963215045</v>
       </c>
       <c r="AI18" t="n">
-        <v>1171.526610699623</v>
+        <v>217.0238316634856</v>
       </c>
       <c r="AJ18" t="n">
-        <v>2218.765582911176</v>
+        <v>757.4819710199459</v>
       </c>
       <c r="AK18" t="n">
-        <v>6.796286281190197</v>
+        <v>4.323981626854378</v>
       </c>
       <c r="AL18" t="n">
-        <v>2.294313885891203</v>
+        <v>1.700946019848965</v>
       </c>
       <c r="AM18" t="n">
-        <v>0.3167975100674</v>
+        <v>0.2409490623574485</v>
       </c>
       <c r="AN18" t="n">
-        <v>0.7065289525394467</v>
+        <v>0.5675926738985889</v>
       </c>
       <c r="AO18" t="n">
-        <v>0.04458361158018932</v>
+        <v>0.03772618757754352</v>
       </c>
       <c r="AP18" t="n">
-        <v>0.1703226554681902</v>
+        <v>0.04486492641750237</v>
       </c>
     </row>
     <row r="19">
@@ -19447,43 +19858,43 @@
         <v>0.1750879373994345</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.5079593006682761</v>
+        <v>0.161734293450243</v>
       </c>
       <c r="AE19" t="n">
-        <v>1172.645024000954</v>
+        <v>384.7301335985855</v>
       </c>
       <c r="AF19" t="n">
-        <v>2138.281429832199</v>
+        <v>396.6920619295927</v>
       </c>
       <c r="AG19" t="n">
-        <v>2396.46791492262</v>
+        <v>467.4644727000749</v>
       </c>
       <c r="AH19" t="n">
-        <v>1578.162055610088</v>
+        <v>813.8566957151378</v>
       </c>
       <c r="AI19" t="n">
-        <v>1170.009785775367</v>
+        <v>211.681060854935</v>
       </c>
       <c r="AJ19" t="n">
-        <v>2170.060361814114</v>
+        <v>552.6950938910098</v>
       </c>
       <c r="AK19" t="n">
-        <v>6.771353143318334</v>
+        <v>4.202707109620146</v>
       </c>
       <c r="AL19" t="n">
-        <v>2.214317436956726</v>
+        <v>1.565067658378571</v>
       </c>
       <c r="AM19" t="n">
-        <v>0.3148940126746722</v>
+        <v>0.2352339373778849</v>
       </c>
       <c r="AN19" t="n">
-        <v>0.6821872197197784</v>
+        <v>0.5334375417022894</v>
       </c>
       <c r="AO19" t="n">
-        <v>0.05072212141196186</v>
+        <v>0.04440892411332811</v>
       </c>
       <c r="AP19" t="n">
-        <v>0.1750474850448548</v>
+        <v>0.044936267288736</v>
       </c>
     </row>
     <row r="20">
@@ -19581,43 +19992,43 @@
         <v>0.1769138997101105</v>
       </c>
       <c r="AD20" t="n">
-        <v>0.4484950687012397</v>
+        <v>0.1592230896092939</v>
       </c>
       <c r="AE20" t="n">
-        <v>1175.054907599417</v>
+        <v>391.964208818527</v>
       </c>
       <c r="AF20" t="n">
-        <v>2165.464204759148</v>
+        <v>432.7641207781085</v>
       </c>
       <c r="AG20" t="n">
-        <v>2396.46791492262</v>
+        <v>467.4644727000749</v>
       </c>
       <c r="AH20" t="n">
-        <v>1564.625688904452</v>
+        <v>810.7899802550767</v>
       </c>
       <c r="AI20" t="n">
-        <v>1182.655011026648</v>
+        <v>216.4604539023937</v>
       </c>
       <c r="AJ20" t="n">
-        <v>2174.690461340442</v>
+        <v>500.8726075575935</v>
       </c>
       <c r="AK20" t="n">
-        <v>6.822448692262152</v>
+        <v>4.291411922577738</v>
       </c>
       <c r="AL20" t="n">
-        <v>2.302126417414333</v>
+        <v>1.701935519158792</v>
       </c>
       <c r="AM20" t="n">
-        <v>0.3256615067701371</v>
+        <v>0.2495452688484334</v>
       </c>
       <c r="AN20" t="n">
-        <v>0.6923830389446824</v>
+        <v>0.547105772536325</v>
       </c>
       <c r="AO20" t="n">
-        <v>0.04547196461374302</v>
+        <v>0.03826782183103732</v>
       </c>
       <c r="AP20" t="n">
-        <v>0.1768769853161549</v>
+        <v>0.06995525004702867</v>
       </c>
     </row>
     <row r="21">
@@ -19715,43 +20126,43 @@
         <v>0.1764563978547965</v>
       </c>
       <c r="AD21" t="n">
-        <v>0.4863679133968036</v>
+        <v>0.1594470743480702</v>
       </c>
       <c r="AE21" t="n">
-        <v>1167.655682181899</v>
+        <v>390.2713231531164</v>
       </c>
       <c r="AF21" t="n">
-        <v>2137.103638180532</v>
+        <v>361.6497982381827</v>
       </c>
       <c r="AG21" t="n">
-        <v>2396.46791492262</v>
+        <v>467.4644727000749</v>
       </c>
       <c r="AH21" t="n">
-        <v>1552.332892806679</v>
+        <v>804.8831657671595</v>
       </c>
       <c r="AI21" t="n">
-        <v>1166.432074468111</v>
+        <v>208.9519187565009</v>
       </c>
       <c r="AJ21" t="n">
-        <v>2153.519990963594</v>
+        <v>487.0310413495528</v>
       </c>
       <c r="AK21" t="n">
-        <v>6.657416559780061</v>
+        <v>4.065198264448886</v>
       </c>
       <c r="AL21" t="n">
-        <v>2.200279969070592</v>
+        <v>1.54317019815041</v>
       </c>
       <c r="AM21" t="n">
-        <v>0.3077340504157632</v>
+        <v>0.2313656715425294</v>
       </c>
       <c r="AN21" t="n">
-        <v>0.672547099055717</v>
+        <v>0.5293554960182081</v>
       </c>
       <c r="AO21" t="n">
-        <v>0.04887524849853255</v>
+        <v>0.04178268629621495</v>
       </c>
       <c r="AP21" t="n">
-        <v>0.1764156061081543</v>
+        <v>0.0451042124543742</v>
       </c>
     </row>
   </sheetData>
@@ -21301,43 +21712,43 @@
         <v>3.63511914452108</v>
       </c>
       <c r="AD2" t="n">
-        <v>4.310849861348289</v>
+        <v>1.162264246805131</v>
       </c>
       <c r="AE2" t="n">
-        <v>5.79278467072074</v>
+        <v>5.560019514024806</v>
       </c>
       <c r="AF2" t="n">
-        <v>349.4331594922516</v>
+        <v>122.768653564983</v>
       </c>
       <c r="AG2" t="n">
-        <v>3494.8440318784</v>
+        <v>3360.869963217549</v>
       </c>
       <c r="AH2" t="n">
-        <v>1814.18137754411</v>
+        <v>1262.633475863294</v>
       </c>
       <c r="AI2" t="n">
-        <v>33.51772433195656</v>
+        <v>7.421737879785495</v>
       </c>
       <c r="AJ2" t="n">
-        <v>4.133081606343394</v>
+        <v>3.947311012139542</v>
       </c>
       <c r="AK2" t="n">
-        <v>1.515862785444546</v>
+        <v>1.261554012355148</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.7340012681887673</v>
+        <v>0.6595434686329512</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.8637873930834047</v>
+        <v>0.7561940934029691</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.7748579719358629</v>
+        <v>0.726017301485074</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.7405824009823327</v>
+        <v>0.6738068459549961</v>
       </c>
       <c r="AP2" t="n">
-        <v>3.614033336049892</v>
+        <v>0.7063055496578282</v>
       </c>
     </row>
     <row r="3">
@@ -21435,43 +21846,43 @@
         <v>3.590855959057254</v>
       </c>
       <c r="AD3" t="n">
-        <v>4.384640618949425</v>
+        <v>1.180321192332656</v>
       </c>
       <c r="AE3" t="n">
-        <v>3.848289933397186</v>
+        <v>3.508641345508761</v>
       </c>
       <c r="AF3" t="n">
-        <v>347.9949171628779</v>
+        <v>122.7929026980866</v>
       </c>
       <c r="AG3" t="n">
-        <v>3494.8440318784</v>
+        <v>3360.869963217549</v>
       </c>
       <c r="AH3" t="n">
-        <v>1813.954037752538</v>
+        <v>1266.996363429176</v>
       </c>
       <c r="AI3" t="n">
-        <v>33.43110354783111</v>
+        <v>7.430249353907502</v>
       </c>
       <c r="AJ3" t="n">
-        <v>2.082937594836802</v>
+        <v>1.63197883648362</v>
       </c>
       <c r="AK3" t="n">
-        <v>1.520716260653602</v>
+        <v>1.269262691507989</v>
       </c>
       <c r="AL3" t="n">
-        <v>0.7244540637823822</v>
+        <v>0.6491165325742583</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.8503511317123591</v>
+        <v>0.7429351223833037</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.7726704324317801</v>
+        <v>0.7237645078432202</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.7468615396971675</v>
+        <v>0.6808891843567177</v>
       </c>
       <c r="AP3" t="n">
-        <v>3.570031963930742</v>
+        <v>0.6998560942348385</v>
       </c>
     </row>
     <row r="4">
@@ -21569,43 +21980,43 @@
         <v>3.695273597792309</v>
       </c>
       <c r="AD4" t="n">
-        <v>4.420436030378218</v>
+        <v>1.189623463436637</v>
       </c>
       <c r="AE4" t="n">
-        <v>1.93363599248161</v>
+        <v>1.000912181842025</v>
       </c>
       <c r="AF4" t="n">
-        <v>351.6339565545468</v>
+        <v>125.3168171102235</v>
       </c>
       <c r="AG4" t="n">
-        <v>3494.8440318784</v>
+        <v>3360.869963217549</v>
       </c>
       <c r="AH4" t="n">
-        <v>1860.901541509482</v>
+        <v>1293.459699280186</v>
       </c>
       <c r="AI4" t="n">
-        <v>34.80585753270905</v>
+        <v>7.728677146576411</v>
       </c>
       <c r="AJ4" t="n">
-        <v>2.306940926423347</v>
+        <v>1.937780656444265</v>
       </c>
       <c r="AK4" t="n">
-        <v>1.563118915501478</v>
+        <v>1.305966549254238</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.7588899557159853</v>
+        <v>0.6832143801439589</v>
       </c>
       <c r="AM4" t="n">
-        <v>0.8892015069739104</v>
+        <v>0.777811876071564</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.7969731978764486</v>
+        <v>0.7476128868964177</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.7664447516724296</v>
+        <v>0.6998597919506693</v>
       </c>
       <c r="AP4" t="n">
-        <v>3.673819316244001</v>
+        <v>0.7096268500426569</v>
       </c>
     </row>
     <row r="5">
@@ -21703,43 +22114,43 @@
         <v>3.687379287968199</v>
       </c>
       <c r="AD5" t="n">
-        <v>4.167334823323447</v>
+        <v>1.126241874982204</v>
       </c>
       <c r="AE5" t="n">
-        <v>1.928058216505245</v>
+        <v>1.018821842883591</v>
       </c>
       <c r="AF5" t="n">
-        <v>355.8415374699192</v>
+        <v>127.194864164186</v>
       </c>
       <c r="AG5" t="n">
-        <v>3494.8440318784</v>
+        <v>3360.869963217549</v>
       </c>
       <c r="AH5" t="n">
-        <v>1848.860454885024</v>
+        <v>1298.611019020658</v>
       </c>
       <c r="AI5" t="n">
-        <v>34.43261770125828</v>
+        <v>7.709636098001313</v>
       </c>
       <c r="AJ5" t="n">
-        <v>2.583524431629171</v>
+        <v>2.295421340395443</v>
       </c>
       <c r="AK5" t="n">
-        <v>1.550515326003251</v>
+        <v>1.295089492020795</v>
       </c>
       <c r="AL5" t="n">
-        <v>0.7597187995662145</v>
+        <v>0.6840762472024707</v>
       </c>
       <c r="AM5" t="n">
-        <v>0.8729114067304686</v>
+        <v>0.7646049967019285</v>
       </c>
       <c r="AN5" t="n">
-        <v>0.7836380924989667</v>
+        <v>0.735320204156135</v>
       </c>
       <c r="AO5" t="n">
-        <v>0.7671728752419564</v>
+        <v>0.701056230514435</v>
       </c>
       <c r="AP5" t="n">
-        <v>3.66597850093768</v>
+        <v>0.711402567250958</v>
       </c>
     </row>
     <row r="6">
@@ -21837,43 +22248,43 @@
         <v>3.660260050526333</v>
       </c>
       <c r="AD6" t="n">
-        <v>4.177660414211473</v>
+        <v>1.125650815588447</v>
       </c>
       <c r="AE6" t="n">
-        <v>1.943673197241472</v>
+        <v>1.017136379799526</v>
       </c>
       <c r="AF6" t="n">
-        <v>351.2263165169414</v>
+        <v>123.9847872926721</v>
       </c>
       <c r="AG6" t="n">
-        <v>3494.8440318784</v>
+        <v>3360.869963217549</v>
       </c>
       <c r="AH6" t="n">
-        <v>1828.035083032504</v>
+        <v>1270.816332874892</v>
       </c>
       <c r="AI6" t="n">
-        <v>34.21461636363728</v>
+        <v>7.608558935088382</v>
       </c>
       <c r="AJ6" t="n">
-        <v>1.966109823816679</v>
+        <v>1.598284946639324</v>
       </c>
       <c r="AK6" t="n">
-        <v>1.533575607467014</v>
+        <v>1.279042326778019</v>
       </c>
       <c r="AL6" t="n">
-        <v>0.7385365934077393</v>
+        <v>0.6632048111663146</v>
       </c>
       <c r="AM6" t="n">
-        <v>0.8468605764498519</v>
+        <v>0.7402704780956014</v>
       </c>
       <c r="AN6" t="n">
-        <v>0.7651156832965907</v>
+        <v>0.7172338553691573</v>
       </c>
       <c r="AO6" t="n">
-        <v>0.7543417654773046</v>
+        <v>0.6882439683667685</v>
       </c>
       <c r="AP6" t="n">
-        <v>3.639020558077191</v>
+        <v>0.7078403675707124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>